<commit_message>
Notas de clases previas
</commit_message>
<xml_diff>
--- a/S_03_Clases/06 Pandas/datos.xlsx
+++ b/S_03_Clases/06 Pandas/datos.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -19,16 +19,16 @@
     <t>A</t>
   </si>
   <si>
-    <t>B</t>
+    <t>L</t>
   </si>
   <si>
-    <t>C</t>
+    <t>U</t>
   </si>
   <si>
-    <t>D</t>
+    <t>M</t>
   </si>
   <si>
-    <t>E</t>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -411,172 +411,172 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>0.4233164631</v>
+        <v>0.4233164630979916</v>
       </c>
       <c r="B2">
-        <v>1.1285162749</v>
+        <v>1.128516274850555</v>
       </c>
       <c r="C2">
-        <v>0.1431947988</v>
+        <v>0.1431947987728295</v>
       </c>
       <c r="D2">
-        <v>-1.4123645347</v>
+        <v>-1.41236453473537</v>
       </c>
       <c r="E2">
-        <v>0.9487793268</v>
+        <v>0.9487793268361908</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>0.9889028572</v>
+        <v>0.9889028572022224</v>
       </c>
       <c r="B3">
-        <v>-1.8222896826</v>
+        <v>-1.822289682647148</v>
       </c>
       <c r="C3">
-        <v>0.8897230283000001</v>
+        <v>0.8897230282691831</v>
       </c>
       <c r="D3">
-        <v>-0.9967536973000001</v>
+        <v>-0.9967536973471972</v>
       </c>
       <c r="E3">
-        <v>-0.9518928277000001</v>
+        <v>-0.951892827650184</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>-0.0628583248</v>
+        <v>-0.06285832484010689</v>
       </c>
       <c r="B4">
-        <v>-0.5879663873000001</v>
+        <v>-0.587966387259811</v>
       </c>
       <c r="C4">
-        <v>-0.5436270186000001</v>
+        <v>-0.5436270185561874</v>
       </c>
       <c r="D4">
-        <v>-0.3845884974</v>
+        <v>-0.3845884973810081</v>
       </c>
       <c r="E4">
-        <v>1.2622425425</v>
+        <v>1.262242542462966</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
-        <v>2.0891302009</v>
+        <v>2.089130200928322</v>
       </c>
       <c r="B5">
-        <v>-0.5002712275</v>
+        <v>-0.5002712275417545</v>
       </c>
       <c r="C5">
-        <v>-1.0906795697</v>
+        <v>-1.090679569698155</v>
       </c>
       <c r="D5">
-        <v>-0.335302698</v>
+        <v>-0.3353026979806761</v>
       </c>
       <c r="E5">
-        <v>-1.0621435193</v>
+        <v>-1.062143519259482</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>-1.081332878</v>
+        <v>-1.081332878046013</v>
       </c>
       <c r="B6">
-        <v>-1.5902703861</v>
+        <v>-1.590270386148148</v>
       </c>
       <c r="C6">
-        <v>1.3557496674</v>
+        <v>1.355749667425276</v>
       </c>
       <c r="D6">
-        <v>-0.348654116</v>
+        <v>-0.348654115996958</v>
       </c>
       <c r="E6">
-        <v>-0.4652896269</v>
+        <v>-0.4652896269021505</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>0.0133058809</v>
+        <v>0.0133058808526776</v>
       </c>
       <c r="B7">
-        <v>0.1767885349</v>
+        <v>0.1767885348951624</v>
       </c>
       <c r="C7">
-        <v>-1.2377863932</v>
+        <v>-1.237786393230702</v>
       </c>
       <c r="D7">
-        <v>-0.4119096261</v>
+        <v>-0.4119096260920766</v>
       </c>
       <c r="E7">
-        <v>2.2849142188</v>
+        <v>2.284914218842941</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <v>-0.3063111051</v>
+        <v>-0.3063111050674059</v>
       </c>
       <c r="B8">
-        <v>2.0236902337</v>
+        <v>2.023690233726497</v>
       </c>
       <c r="C8">
-        <v>0.9127223026</v>
+        <v>0.91272230261041</v>
       </c>
       <c r="D8">
-        <v>0.4743388227</v>
+        <v>0.4743388227124177</v>
       </c>
       <c r="E8">
-        <v>0.6567092771</v>
+        <v>0.65670927708812</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
-        <v>0.562534575</v>
+        <v>0.5625345749784322</v>
       </c>
       <c r="B9">
-        <v>0.0288412741</v>
+        <v>0.0288412741344594</v>
       </c>
       <c r="C9">
-        <v>-1.1269611471</v>
+        <v>-1.126961147145649</v>
       </c>
       <c r="D9">
-        <v>0.2464037076</v>
+        <v>0.2464037075798208</v>
       </c>
       <c r="E9">
-        <v>1.1754914558</v>
+        <v>1.175491455761141</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>-0.6522870633</v>
+        <v>-0.6522870633031013</v>
       </c>
       <c r="B10">
-        <v>0.9822288854000001</v>
+        <v>0.9822288853780358</v>
       </c>
       <c r="C10">
-        <v>1.1772809721</v>
+        <v>1.177280972076537</v>
       </c>
       <c r="D10">
-        <v>-0.7352919403</v>
+        <v>-0.7352919403387764</v>
       </c>
       <c r="E10">
-        <v>2.5974023382</v>
+        <v>2.597402338175312</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>0.6949944617</v>
+        <v>0.694994461699469</v>
       </c>
       <c r="B11">
-        <v>-0.5415108223</v>
+        <v>-0.5415108223460028</v>
       </c>
       <c r="C11">
-        <v>-0.0666884078</v>
+        <v>-0.06668840776494429</v>
       </c>
       <c r="D11">
-        <v>0.3350891122</v>
+        <v>0.3350891121534909</v>
       </c>
       <c r="E11">
-        <v>0.3450399445</v>
+        <v>0.3450399444500379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>